<commit_message>
First conceptual design iteration
</commit_message>
<xml_diff>
--- a/2 - Conceptual Design/Weight & Cost Analysis/weight_and_cost_breakdown.xlsx
+++ b/2 - Conceptual Design/Weight & Cost Analysis/weight_and_cost_breakdown.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaros\Documents\GitHub\DISECON_PIA\2 - Conceptual Design\Weight &amp; Cost Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90CA6D7-B16D-4AB1-8538-CF9953836F41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23409FEE-3F80-408A-A86D-37FD9170AF45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2220" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$3:$J$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$3:$I$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$3:$I$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Note</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Power module</t>
   </si>
   <si>
-    <t>Payload</t>
-  </si>
-  <si>
     <t>Main gear wheel</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Source</t>
   </si>
   <si>
-    <t>https://hobbyking.com/es_es/turnigy-high-capacity-16000mah-4s-12c-multi-rotor-lipo-pack-w-xt90.html</t>
-  </si>
-  <si>
     <t>Autopilot</t>
   </si>
   <si>
@@ -177,18 +171,9 @@
     <t>https://es.aliexpress.com/item/32473796463.html?spm=a2g0s.9042311.0.0.37de63c0dJBzZb</t>
   </si>
   <si>
-    <t>https://es.aliexpress.com/item/32880128406.html?spm=a2g0s.9042311.0.0.37de63c0dJBzZb</t>
-  </si>
-  <si>
     <t>https://es.aliexpress.com/item/4000378054837.html?spm=a2g0s.9042311.0.0.37de63c0dJBzZb</t>
   </si>
   <si>
-    <t>https://hobbyking.com/es_es/aerostar-rvs-80a-electronic-speed-controller-w-reverse-function-5a-bec-2-6s.html</t>
-  </si>
-  <si>
-    <t>https://shop.holybro.com/c/915mhz_0471</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -199,6 +184,18 @@
   </si>
   <si>
     <t>https://hobbyking.com/en_us/propdrive-v2-5050-580kv-brushless-outrunner-motor.html?queryID=6e8d3410b6e69ca2706017e9bbc57584&amp;objectID=59101&amp;indexName=hbk_live_magento_en_us_products_hbk_price_stock_2_group_1_asc</t>
+  </si>
+  <si>
+    <t>https://www.flir.com/products/xt2/</t>
+  </si>
+  <si>
+    <t>https://www.kopterworx.com/pixhawk-rfd868-ultra-long-range-telemetry-modem-bundle.html</t>
+  </si>
+  <si>
+    <t>https://rcbattery.com/liperior-13000mah-6s-12c-22-2v-lipo-battery-with-xt90-plug.html</t>
+  </si>
+  <si>
+    <t>https://hobbyking.com/en_us/yep-120a-lv-2-6s-brushless-speed-controller-with-selectable-sbec.html?queryID=21051a358b501dd4afd35bbe7caa9e8c&amp;objectID=40131&amp;indexName=hbk_live_magento_en_us_products</t>
   </si>
 </sst>
 </file>
@@ -209,7 +206,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,13 +235,54 @@
       <family val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Palatino Linotype"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Palatino Linotype"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,8 +301,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -324,17 +377,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -345,12 +416,64 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -362,9 +485,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -379,6 +515,23 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -420,11 +573,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -439,9 +592,42 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -454,11 +640,6 @@
           <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -758,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +961,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="3">
         <v>19.93</v>
@@ -808,7 +989,7 @@
     </row>
     <row r="3" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -835,31 +1016,31 @@
         <v>7</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -868,33 +1049,33 @@
         <v>3.1E-2</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" ref="E5:E32" si="0">C5*D5</f>
+        <f t="shared" ref="E5:E11" si="0">C5*D5</f>
         <v>3.1E-2</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>34.56</v>
       </c>
-      <c r="G5" s="11">
-        <f t="shared" ref="G5:G32" si="1">$B$1*F5</f>
+      <c r="G5" s="10">
+        <f t="shared" ref="G5:G11" si="1">$B$1*F5</f>
         <v>688.7808</v>
       </c>
-      <c r="H5" s="11">
-        <f t="shared" ref="H5:H32" si="2">C5*F5</f>
+      <c r="H5" s="10">
+        <f t="shared" ref="H5:H11" si="2">C5*F5</f>
         <v>34.56</v>
       </c>
-      <c r="I5" s="11">
-        <f t="shared" ref="I5:I32" si="3">C5*G5</f>
+      <c r="I5" s="10">
+        <f t="shared" ref="I5:I11" si="3">C5*G5</f>
         <v>688.7808</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="3">
@@ -907,66 +1088,66 @@
         <f t="shared" si="0"/>
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>211</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <f t="shared" si="1"/>
         <v>4205.2299999999996</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <f t="shared" si="2"/>
         <v>211</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <f t="shared" si="3"/>
         <v>4205.2299999999996</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
       <c r="D7" s="3">
-        <v>1.41</v>
+        <v>1.5229999999999999</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>1.41</v>
-      </c>
-      <c r="F7" s="11">
-        <v>189.99</v>
-      </c>
-      <c r="G7" s="11">
+        <v>1.5229999999999999</v>
+      </c>
+      <c r="F7" s="10">
+        <v>109.99</v>
+      </c>
+      <c r="G7" s="10">
         <f t="shared" si="1"/>
-        <v>3786.5007000000001</v>
-      </c>
-      <c r="H7" s="11">
+        <v>2192.1007</v>
+      </c>
+      <c r="H7" s="10">
         <f t="shared" si="2"/>
-        <v>189.99</v>
-      </c>
-      <c r="I7" s="11">
+        <v>109.99</v>
+      </c>
+      <c r="I7" s="10">
         <f t="shared" si="3"/>
-        <v>3786.5007000000001</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>40</v>
+        <v>2192.1007</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3">
@@ -979,155 +1160,153 @@
         <f t="shared" si="0"/>
         <v>0.33100000000000002</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>47.95</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <f t="shared" si="1"/>
         <v>955.64350000000002</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <f t="shared" si="2"/>
         <v>47.95</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <f t="shared" si="3"/>
         <v>955.64350000000002</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>53</v>
+      <c r="J8" s="17" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>0.03</v>
+        <v>0.63900000000000001</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-      <c r="F9" s="11">
-        <v>14.04</v>
-      </c>
-      <c r="G9" s="11">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
         <f t="shared" si="1"/>
-        <v>279.81719999999996</v>
-      </c>
-      <c r="H9" s="11">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
         <f t="shared" si="2"/>
-        <v>14.04</v>
-      </c>
-      <c r="I9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
         <f t="shared" si="3"/>
-        <v>279.81719999999996</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>46</v>
+        <v>0</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3">
-        <v>8.5000000000000006E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="F10" s="10">
+        <v>83</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="1"/>
+        <v>1654.19</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="2"/>
+        <v>83</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="3"/>
+        <v>1654.19</v>
+      </c>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="F10" s="11">
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="F11" s="10">
         <v>81.760000000000005</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G11" s="10">
         <f t="shared" si="1"/>
         <v>1629.4768000000001</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H11" s="10">
         <f t="shared" si="2"/>
         <v>81.760000000000005</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I11" s="10">
         <f t="shared" si="3"/>
         <v>1629.4768000000001</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0</v>
-      </c>
-      <c r="G12" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -1136,106 +1315,106 @@
         <v>0</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="11">
-        <v>0</v>
-      </c>
-      <c r="G13" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E13:E25" si="4">C13*D13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" ref="G13:G25" si="5">$B$1*F13</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" ref="H13:H25" si="6">C13*F13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" ref="I13:I25" si="7">C13*G13</f>
         <v>0</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>3.3000000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="0"/>
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
-      <c r="G14" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="11">
-        <v>0</v>
-      </c>
-      <c r="G15" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1244,34 +1423,34 @@
         <v>0</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="11">
-        <v>0</v>
-      </c>
-      <c r="G16" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1280,176 +1459,178 @@
         <v>0</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="11">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>37</v>
+      <c r="B18" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C18" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="3">
         <v>0</v>
       </c>
       <c r="E18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0</v>
-      </c>
-      <c r="G18" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="C19" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="3">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
-      </c>
-      <c r="F19" s="11">
-        <v>83</v>
-      </c>
-      <c r="G19" s="11">
-        <f t="shared" si="1"/>
-        <v>1654.19</v>
-      </c>
-      <c r="H19" s="11">
-        <f t="shared" si="2"/>
-        <v>83</v>
-      </c>
-      <c r="I19" s="11">
-        <f t="shared" si="3"/>
-        <v>1654.19</v>
-      </c>
-      <c r="J19" s="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="20" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="E20" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="3">
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>8.2000000000000003E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" si="0"/>
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="F21" s="11">
-        <v>37.270000000000003</v>
-      </c>
-      <c r="G21" s="11">
-        <f t="shared" si="1"/>
-        <v>742.79110000000003</v>
-      </c>
-      <c r="H21" s="11">
-        <f t="shared" si="2"/>
-        <v>37.270000000000003</v>
-      </c>
-      <c r="I21" s="11">
-        <f t="shared" si="3"/>
-        <v>742.79110000000003</v>
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="10">
+        <v>66.97</v>
+      </c>
+      <c r="G21" s="10">
+        <f t="shared" si="5"/>
+        <v>1334.7121</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="6"/>
+        <v>66.97</v>
+      </c>
+      <c r="I21" s="10">
+        <f t="shared" si="7"/>
+        <v>1334.7121</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -1458,34 +1639,34 @@
         <v>0</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="11">
-        <v>0</v>
-      </c>
-      <c r="G22" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="10">
+        <v>0</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="3">
         <v>1</v>
@@ -1494,228 +1675,228 @@
         <v>0</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="11">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
       </c>
       <c r="D24" s="3">
-        <v>1</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0</v>
-      </c>
-      <c r="G24" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>2.4E-2</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="3">
         <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>2.4E-2</v>
+        <v>0</v>
       </c>
       <c r="E25" s="3">
-        <f t="shared" si="0"/>
-        <v>2.4E-2</v>
-      </c>
-      <c r="F25" s="11">
-        <v>0</v>
-      </c>
-      <c r="G25" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="3">
-        <v>2</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="11">
-        <v>0</v>
-      </c>
-      <c r="G26" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <f>C27*D27</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
+      <c r="G27" s="10">
+        <f>$B$1*F27</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <f>C27*F27</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <f>C27*G27</f>
+        <v>0</v>
+      </c>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="E28" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="11">
-        <v>0</v>
-      </c>
-      <c r="G28" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="3"/>
+        <f>C28*D28</f>
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="F28" s="10">
+        <v>325.52999999999997</v>
+      </c>
+      <c r="G28" s="10">
+        <f>$B$1*F28</f>
+        <v>6487.812899999999</v>
+      </c>
+      <c r="H28" s="10">
+        <f>C28*F28</f>
+        <v>325.52999999999997</v>
+      </c>
+      <c r="I28" s="10">
+        <f>C28*G28</f>
+        <v>6487.812899999999</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
       </c>
       <c r="D29" s="3">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E29" s="3">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
-      </c>
-      <c r="F29" s="11">
-        <v>39</v>
-      </c>
-      <c r="G29" s="11">
-        <f t="shared" si="1"/>
-        <v>777.27</v>
-      </c>
-      <c r="H29" s="11">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="I29" s="11">
-        <f t="shared" si="3"/>
-        <v>777.27</v>
+        <f>C29*D29</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <f>$B$1*F29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
+        <f>C29*F29</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
+        <f>C29*G29</f>
+        <v>0</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>9</v>
       </c>
       <c r="C30" s="3">
         <v>1</v>
@@ -1724,35 +1905,35 @@
         <v>0</v>
       </c>
       <c r="E30" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="11">
-        <v>0</v>
-      </c>
-      <c r="G30" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="11">
-        <f t="shared" si="3"/>
+        <f>C30*D30</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10">
+        <f>$B$1*F30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <f>C30*F30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="10">
+        <f>C30*G30</f>
         <v>0</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="C31" s="3">
         <v>1</v>
       </c>
@@ -1760,86 +1941,62 @@
         <v>0</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="11">
-        <v>0</v>
-      </c>
-      <c r="G31" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="11">
-        <f t="shared" si="3"/>
+        <f>C31*D31</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <f>$B$1*F31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="10">
+        <f>C31*F31</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="10">
+        <f>C31*G31</f>
         <v>0</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="3">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="11">
-        <v>0</v>
-      </c>
-      <c r="G32" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="7">
+        <f>SUM(E4:E31)</f>
+        <v>2.9957999999999996</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="17.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E33" s="8">
-        <f>SUM(E4:E32)</f>
-        <v>3.1292999999999997</v>
-      </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="12">
-        <f>SUM(H4:H32)</f>
-        <v>738.57</v>
-      </c>
-      <c r="I33" s="5">
-        <f>SUM(I4:I32)</f>
-        <v>14719.700100000002</v>
-      </c>
-      <c r="J33" s="7"/>
+        <f>SUM(H4:H31)</f>
+        <v>960.76</v>
+      </c>
+      <c r="I32" s="4">
+        <f>SUM(I4:I31)</f>
+        <v>19147.946799999998</v>
+      </c>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
@@ -2009,54 +2166,71 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-    </row>
   </sheetData>
   <autoFilter ref="A3:J3" xr:uid="{ABA105E2-361E-4C17-8FC0-1FD0BE18A29B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J36">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J32">
       <sortCondition ref="A3"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="CAD model">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="CAD model">
       <formula>NOT(ISERROR(SEARCH("CAD model",B7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="CAD model">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="CAD model">
       <formula>NOT(ISERROR(SEARCH("CAD model",B7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Supplier data">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Supplier data">
       <formula>NOT(ISERROR(SEARCH("Supplier data",B5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B32">
-    <cfRule type="containsText" dxfId="6" priority="74" operator="containsText" text="CAD model">
+  <conditionalFormatting sqref="B4:B9">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="CAD model">
       <formula>NOT(ISERROR(SEARCH("CAD model",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="75" operator="containsText" text="Supplier data">
+    <cfRule type="duplicateValues" dxfId="20" priority="6"/>
+    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="CAD model">
+      <formula>NOT(ISERROR(SEARCH("CAD model",B4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B13">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Measured">
+      <formula>NOT(ISERROR(SEARCH("Measured",B10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16:B31">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="Supplier data">
+      <formula>NOT(ISERROR(SEARCH("Supplier data",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B15">
+    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="Rough estimate">
+      <formula>NOT(ISERROR(SEARCH("Rough estimate",B14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="Supplier data">
+      <formula>NOT(ISERROR(SEARCH("Supplier data",B12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B31">
+    <cfRule type="containsText" dxfId="14" priority="92" operator="containsText" text="CAD model">
+      <formula>NOT(ISERROR(SEARCH("CAD model",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="93" operator="containsText" text="Supplier data">
       <formula>NOT(ISERROR(SEARCH("Supplier data",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="76" operator="containsText" text="Rough estimate">
+    <cfRule type="containsText" dxfId="12" priority="94" operator="containsText" text="Rough estimate">
       <formula>NOT(ISERROR(SEARCH("Rough estimate",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="77" operator="containsText" text="Measured">
+    <cfRule type="containsText" dxfId="11" priority="95" operator="containsText" text="Measured">
       <formula>NOT(ISERROR(SEARCH("Measured",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="78" operator="containsText" text="Supplier data">
+    <cfRule type="containsText" dxfId="10" priority="96" operator="containsText" text="Supplier data">
       <formula>NOT(ISERROR(SEARCH("Supplier data",B4)))</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="79">
+    <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2066,33 +2240,45 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="80" operator="containsText" text="S$J$13">
+    <cfRule type="containsText" dxfId="9" priority="98" operator="containsText" text="S$J$13">
       <formula>NOT(ISERROR(SEARCH("S$J$13",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="81" operator="containsText" text="Supplier data">
+    <cfRule type="containsText" dxfId="8" priority="99" operator="containsText" text="Supplier data">
+      <formula>NOT(ISERROR(SEARCH("Supplier data",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Measured">
+      <formula>NOT(ISERROR(SEARCH("Measured",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Rough estimate">
+      <formula>NOT(ISERROR(SEARCH("Rough estimate",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Supplier data">
       <formula>NOT(ISERROR(SEARCH("Supplier data",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J25" r:id="rId1" xr:uid="{1D7A48B2-9A72-49C6-9452-BA9AD04BF0B6}"/>
+    <hyperlink ref="J24" r:id="rId1" xr:uid="{1D7A48B2-9A72-49C6-9452-BA9AD04BF0B6}"/>
+    <hyperlink ref="J8" r:id="rId2" xr:uid="{3F6EE08C-93D8-45A9-B933-68A4DE6E8096}"/>
+    <hyperlink ref="J9" r:id="rId3" xr:uid="{DD755EDD-41E6-477F-B6DA-3AEF687EB1B2}"/>
+    <hyperlink ref="J7" r:id="rId4" xr:uid="{163D9CDB-ABB1-444E-AD5F-01B17D8616CF}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="76" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup scale="76" fitToHeight="0" orientation="landscape" r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="64" operator="containsText" id="{CD70BEBB-0554-42E1-A6B9-490442AF65AE}">
-            <xm:f>NOT(ISERROR(SEARCH($B$18,B4)))</xm:f>
-            <xm:f>$B$18</xm:f>
+          <x14:cfRule type="containsText" priority="108" operator="containsText" id="{CD70BEBB-0554-42E1-A6B9-490442AF65AE}">
+            <xm:f>NOT(ISERROR(SEARCH($B$17,B4)))</xm:f>
+            <xm:f>$B$17</xm:f>
             <x14:dxf>
               <font>
                 <color theme="5" tint="-0.499984740745262"/>
               </font>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="65" operator="containsText" id="{076B74B2-7ACA-49AB-8B02-8386556C916E}">
+          <x14:cfRule type="containsText" priority="109" operator="containsText" id="{076B74B2-7ACA-49AB-8B02-8386556C916E}">
             <xm:f>NOT(ISERROR(SEARCH($B$7,B4)))</xm:f>
             <xm:f>$B$7</xm:f>
             <x14:dxf>
@@ -2106,9 +2292,9 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="66" operator="containsText" id="{B9317E1A-C086-4B70-8618-80193286E9F2}">
-            <xm:f>NOT(ISERROR(SEARCH($B$16,B4)))</xm:f>
-            <xm:f>$B$16</xm:f>
+          <x14:cfRule type="containsText" priority="110" operator="containsText" id="{B9317E1A-C086-4B70-8618-80193286E9F2}">
+            <xm:f>NOT(ISERROR(SEARCH($B$15,B4)))</xm:f>
+            <xm:f>$B$15</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -2117,9 +2303,9 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="67" operator="containsText" id="{C9EE5F59-2E2F-4938-8ED6-2FBE7ED8CB1F}">
-            <xm:f>NOT(ISERROR(SEARCH($B$24,B4)))</xm:f>
-            <xm:f>$B$24</xm:f>
+          <x14:cfRule type="containsText" priority="111" operator="containsText" id="{C9EE5F59-2E2F-4938-8ED6-2FBE7ED8CB1F}">
+            <xm:f>NOT(ISERROR(SEARCH($B$23,B4)))</xm:f>
+            <xm:f>$B$23</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -2131,9 +2317,9 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="68" operator="containsText" id="{420E6EE1-6DA5-4092-99BF-39FB8567E1D1}">
-            <xm:f>NOT(ISERROR(SEARCH($B$13,B4)))</xm:f>
-            <xm:f>$B$13</xm:f>
+          <x14:cfRule type="containsText" priority="112" operator="containsText" id="{420E6EE1-6DA5-4092-99BF-39FB8567E1D1}">
+            <xm:f>NOT(ISERROR(SEARCH(#REF!,B4)))</xm:f>
+            <xm:f>#REF!</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF006100"/>
@@ -2145,7 +2331,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B4:B32</xm:sqref>
+          <xm:sqref>B4:B31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>